<commit_message>
Update lab3 excel paths
</commit_message>
<xml_diff>
--- a/Docs/lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/lab3/Lab03_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB611B9C-05A5-EA4D-BA75-FD3E7E243620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7F6BEA-08A4-B344-B692-C41276A9FBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="97">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -72,27 +72,6 @@
     <t>Student 3:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">F02. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>cautarea filmelor care au un anumit regizor (sau parti din numele regizorului).</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">F02. Covered source code </t>
   </si>
   <si>
@@ -153,13 +132,7 @@
     <t>F02_P01</t>
   </si>
   <si>
-    <t>1 - 2(F) - …</t>
-  </si>
-  <si>
     <t>F02_P02</t>
-  </si>
-  <si>
-    <t>1 - 2(T) - …</t>
   </si>
   <si>
     <t>F02_P03</t>
@@ -501,24 +474,45 @@
   <si>
     <t>nu e nevoie</t>
   </si>
+  <si>
+    <t>1 - 2(T) - 3</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 4(T) - 5(T) - 6 - 4(F) - 3</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 4(T) - 5(T) - 6 - 4(T) - 5(F) - 4(F) - 3</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 4(T) - 5(T) - 6 - 4(T) - 5(T) - 6 - 4(F) - 3</t>
+  </si>
+  <si>
+    <t>F02_P04</t>
+  </si>
+  <si>
+    <t>F02_P05</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 4(T) - 5(F) - 4(F) - 3</t>
+  </si>
+  <si>
+    <t>F02_P06</t>
+  </si>
+  <si>
+    <t>1 - 2(F) - 4(T) - 5(F) - 6 - 4(T) - 5(F) - 6 - 4(F) - 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1185,84 +1179,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1274,15 +1268,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1291,197 +1285,203 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1975,7 +1975,7 @@
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1988,15 +1988,15 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B11" s="107" t="s">
-        <v>87</v>
+      <c r="B11" s="106" t="s">
+        <v>84</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2030,13 +2030,14 @@
   <dimension ref="B1:T24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="17" max="17" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.2">
@@ -2051,22 +2052,22 @@
       <c r="I1" s="42"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B3" s="108" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="48"/>
+      <c r="B3" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="47"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" s="40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
@@ -2074,7 +2075,7 @@
       <c r="F6" s="32"/>
       <c r="G6" s="32"/>
       <c r="I6" s="40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="41"/>
       <c r="K6" s="41"/>
@@ -2083,7 +2084,7 @@
       <c r="N6" s="41"/>
       <c r="O6" s="41"/>
       <c r="Q6" s="40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R6" s="41"/>
       <c r="S6" s="41"/>
@@ -2091,18 +2092,18 @@
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B8" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
       <c r="I8" s="12"/>
       <c r="Q8" s="45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R8" s="45"/>
       <c r="S8" s="45"/>
@@ -2112,10 +2113,10 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="44"/>
       <c r="E9" s="44"/>
@@ -2123,7 +2124,7 @@
       <c r="G9" s="37"/>
       <c r="I9" s="38"/>
       <c r="Q9" s="45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R9" s="45"/>
       <c r="S9" s="45"/>
@@ -2133,29 +2134,29 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="44"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
-      <c r="I10" s="49" t="s">
+      <c r="I10" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
+      <c r="Q10" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="51"/>
-      <c r="Q10" s="45" t="s">
+      <c r="R10" s="45" t="s">
         <v>24</v>
-      </c>
-      <c r="R10" s="45" t="s">
-        <v>25</v>
       </c>
       <c r="S10" s="45"/>
       <c r="T10" s="35">
@@ -2164,62 +2165,62 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="44"/>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="44"/>
       <c r="E12" s="44"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="54"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="44"/>
       <c r="E13" s="44"/>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="53"/>
       <c r="Q13" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R13" s="41"/>
       <c r="S13" s="41"/>
@@ -2227,174 +2228,176 @@
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B14" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="44"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="54"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="54"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="53"/>
       <c r="Q15" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="58" t="s">
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="53"/>
+      <c r="Q16" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="54"/>
-      <c r="Q16" s="36" t="s">
-        <v>32</v>
-      </c>
       <c r="R16" s="43" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="S16" s="43"/>
       <c r="T16" s="43"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I17" s="52"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="54"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="53"/>
       <c r="Q17" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="R17" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
+        <v>32</v>
+      </c>
+      <c r="R17" s="109" t="s">
+        <v>89</v>
+      </c>
+      <c r="S17" s="110"/>
+      <c r="T17" s="111"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="54"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53"/>
       <c r="Q18" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="R18" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
+        <v>33</v>
+      </c>
+      <c r="R18" s="109" t="s">
+        <v>94</v>
+      </c>
+      <c r="S18" s="110"/>
+      <c r="T18" s="111"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="54"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
       <c r="Q19" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="R19" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="S19" s="43"/>
-      <c r="T19" s="43"/>
+        <v>92</v>
+      </c>
+      <c r="R19" s="109" t="s">
+        <v>90</v>
+      </c>
+      <c r="S19" s="110"/>
+      <c r="T19" s="111"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I20" s="52"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-      <c r="L20" s="53"/>
-      <c r="M20" s="53"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="54"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53"/>
       <c r="Q20" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="R20" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
+        <v>93</v>
+      </c>
+      <c r="R20" s="109" t="s">
+        <v>91</v>
+      </c>
+      <c r="S20" s="110"/>
+      <c r="T20" s="111"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I21" s="52"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="53"/>
-      <c r="O21" s="54"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="53"/>
       <c r="Q21" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="R21" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="S21" s="43"/>
-      <c r="T21" s="43"/>
+        <v>95</v>
+      </c>
+      <c r="R21" s="109" t="s">
+        <v>96</v>
+      </c>
+      <c r="S21" s="110"/>
+      <c r="T21" s="111"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I22" s="52"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="54"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I23" s="52"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="53"/>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="N23" s="53"/>
-      <c r="O23" s="54"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="53"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.2">
-      <c r="I24" s="55"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R20:T20"/>
     <mergeCell ref="D1:I1"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R21:T21"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="I10:O24"/>
@@ -2406,9 +2409,7 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="R18:T18"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="R16:T16"/>
@@ -2431,7 +2432,7 @@
   <dimension ref="B1:AB16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2467,221 +2468,221 @@
       <c r="G1" s="42"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="B3" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
+      <c r="B3" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="2:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
+      <c r="R6" s="64"/>
+      <c r="S6" s="64"/>
+      <c r="T6" s="64"/>
+      <c r="U6" s="64"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="64"/>
+      <c r="AA6" s="64"/>
+      <c r="AB6" s="64"/>
+    </row>
+    <row r="7" spans="2:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="66" t="s">
+      <c r="F7" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="65"/>
-      <c r="AA6" s="65"/>
-      <c r="AB6" s="65"/>
-    </row>
-    <row r="7" spans="2:28" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="62" t="s">
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="63"/>
+    </row>
+    <row r="8" spans="2:28" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="64"/>
+      <c r="C8" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="61"/>
+      <c r="F8" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="63" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="63"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="63"/>
-      <c r="U7" s="63"/>
-      <c r="V7" s="64" t="s">
+      <c r="I8" s="60"/>
+      <c r="J8" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-    </row>
-    <row r="8" spans="2:28" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="65"/>
-      <c r="C8" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="61" t="s">
+      <c r="K8" s="60"/>
+      <c r="L8" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61" t="s">
+      <c r="O8" s="60"/>
+      <c r="P8" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="S8" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="T8" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61" t="s">
+      <c r="V8" s="63">
+        <v>0</v>
+      </c>
+      <c r="W8" s="63">
+        <v>1</v>
+      </c>
+      <c r="X8" s="63">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61" t="s">
+      <c r="Z8" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="61"/>
-      <c r="P8" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q8" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="R8" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="S8" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="T8" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" s="63" t="s">
+      <c r="AA8" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="V8" s="64">
-        <v>0</v>
-      </c>
-      <c r="W8" s="64">
-        <v>1</v>
-      </c>
-      <c r="X8" s="64">
-        <v>2</v>
-      </c>
-      <c r="Y8" s="64" t="s">
+      <c r="AB8" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="Z8" s="64" t="s">
+    </row>
+    <row r="9" spans="2:28" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="64"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AA8" s="64" t="s">
+      <c r="G9" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="AB8" s="64" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:28" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="65"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="H9" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O9" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="63"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="64"/>
+        <v>52</v>
+      </c>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="63"/>
+      <c r="W9" s="63"/>
+      <c r="X9" s="63"/>
+      <c r="Y9" s="63"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="63"/>
     </row>
     <row r="10" spans="2:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -2709,13 +2710,13 @@
     </row>
     <row r="11" spans="2:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="17"/>
@@ -2744,7 +2745,7 @@
     </row>
     <row r="12" spans="2:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
@@ -2775,7 +2776,7 @@
     </row>
     <row r="13" spans="2:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="15"/>
@@ -2806,7 +2807,7 @@
     </row>
     <row r="14" spans="2:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
@@ -2837,7 +2838,7 @@
     </row>
     <row r="15" spans="2:28" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="15"/>
@@ -2943,110 +2944,110 @@
       <c r="G1" s="42"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="93" t="s">
+      <c r="E4" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="103" t="s">
+      <c r="L4" s="95"/>
+    </row>
+    <row r="5" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="93"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="96" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="97"/>
+      <c r="K5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="L5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="96"/>
-      <c r="K4" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" s="96"/>
-    </row>
-    <row r="5" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="94"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="97" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="98"/>
-      <c r="K5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B6" s="23">
         <v>9</v>
       </c>
-      <c r="C6" s="99" t="s">
-        <v>67</v>
+      <c r="C6" s="98" t="s">
+        <v>64</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="105" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="106"/>
+        <v>18</v>
+      </c>
+      <c r="I6" s="104" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="105"/>
       <c r="K6" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="23">
         <v>10</v>
       </c>
-      <c r="C7" s="99"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E7" s="23">
         <v>5</v>
@@ -3055,113 +3056,113 @@
         <v>6</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="96"/>
+        <v>18</v>
+      </c>
+      <c r="I7" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="95"/>
       <c r="K7" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="23">
         <v>11</v>
       </c>
-      <c r="C8" s="99"/>
+      <c r="C8" s="98"/>
       <c r="D8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="96"/>
+        <v>18</v>
+      </c>
+      <c r="I8" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="95"/>
       <c r="K8" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="23">
         <v>12</v>
       </c>
-      <c r="C9" s="99"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="96"/>
+        <v>18</v>
+      </c>
+      <c r="I9" s="94" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="95"/>
       <c r="K9" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="100"/>
+      <c r="C10" s="99"/>
       <c r="D10" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="97" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="98"/>
+        <v>18</v>
+      </c>
+      <c r="I10" s="96" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="97"/>
       <c r="K10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
@@ -3179,88 +3180,88 @@
     </row>
     <row r="12" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="25"/>
+    </row>
+    <row r="13" spans="2:14" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="76"/>
+      <c r="H13" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="2:14" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="84" t="s">
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="84"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="85"/>
-      <c r="F13" s="76" t="s">
+      <c r="N13" s="90"/>
+    </row>
+    <row r="14" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="77"/>
-      <c r="H13" s="84" t="s">
+      <c r="C14" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="86"/>
-      <c r="M13" s="90" t="s">
+      <c r="D14" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="N13" s="91"/>
-    </row>
-    <row r="14" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="68" t="s">
+      <c r="E14" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="F14" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="G14" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="H14" s="79" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="74" t="s">
+      <c r="I14" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="K14" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="78" t="s">
+      <c r="L14" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="80" t="s">
+      <c r="M14" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="70" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="K14" s="82" t="s">
+      <c r="N14" s="78" t="s">
         <v>81</v>
       </c>
-      <c r="L14" s="87" t="s">
-        <v>82</v>
-      </c>
-      <c r="M14" s="89" t="s">
-        <v>83</v>
-      </c>
-      <c r="N14" s="79" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="69"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="73"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="83"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="74"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="73"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="28">
@@ -3272,17 +3273,17 @@
       <c r="D16" s="26">
         <v>0</v>
       </c>
-      <c r="E16" s="109">
+      <c r="E16" s="108">
         <v>1</v>
       </c>
       <c r="F16" s="27">
         <v>0</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I16" s="28">
         <f>SUM(J16:K16)</f>
@@ -3296,7 +3297,7 @@
       </c>
       <c r="L16" s="30"/>
       <c r="M16" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="N16" s="31">
         <f>C16</f>

</xml_diff>